<commit_message>
correction typo closingRepoeningDate (#293) cab6f23c9997deb3fcb0d44b13e703e7baec9cc3
</commit_message>
<xml_diff>
--- a/ig/main/StructureDefinition-ror-healthcareservice.xlsx
+++ b/ig/main/StructureDefinition-ror-healthcareservice.xlsx
@@ -54,7 +54,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-01-15T15:51:45+00:00</t>
+    <t>2024-01-24T08:52:08+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -1988,46 +1988,46 @@
     <t>Service is not available (seasonally or for a public holiday) from this date.</t>
   </si>
   <si>
-    <t>HealthcareService.notAvailable:closingRepoeningDate</t>
-  </si>
-  <si>
-    <t>closingRepoeningDate</t>
+    <t>HealthcareService.notAvailable:closingReopeningDate</t>
+  </si>
+  <si>
+    <t>closingReopeningDate</t>
   </si>
   <si>
     <t>Période de fermeture (during.start) et de réouverture prévisionnelle (during.end).</t>
   </si>
   <si>
-    <t>HealthcareService.notAvailable:closingRepoeningDate.id</t>
-  </si>
-  <si>
-    <t>HealthcareService.notAvailable:closingRepoeningDate.extension</t>
-  </si>
-  <si>
-    <t>HealthcareService.notAvailable:closingRepoeningDate.modifierExtension</t>
-  </si>
-  <si>
-    <t>HealthcareService.notAvailable:closingRepoeningDate.description</t>
+    <t>HealthcareService.notAvailable:closingReopeningDate.id</t>
+  </si>
+  <si>
+    <t>HealthcareService.notAvailable:closingReopeningDate.extension</t>
+  </si>
+  <si>
+    <t>HealthcareService.notAvailable:closingReopeningDate.modifierExtension</t>
+  </si>
+  <si>
+    <t>HealthcareService.notAvailable:closingReopeningDate.description</t>
   </si>
   <si>
     <t>Période de fermeture et de réouverture prévisionnelle</t>
   </si>
   <si>
-    <t>HealthcareService.notAvailable:closingRepoeningDate.during</t>
-  </si>
-  <si>
-    <t>HealthcareService.notAvailable:closingRepoeningDate.during.id</t>
+    <t>HealthcareService.notAvailable:closingReopeningDate.during</t>
+  </si>
+  <si>
+    <t>HealthcareService.notAvailable:closingReopeningDate.during.id</t>
   </si>
   <si>
     <t>HealthcareService.notAvailable.during.id</t>
   </si>
   <si>
-    <t>HealthcareService.notAvailable:closingRepoeningDate.during.extension</t>
+    <t>HealthcareService.notAvailable:closingReopeningDate.during.extension</t>
   </si>
   <si>
     <t>HealthcareService.notAvailable.during.extension</t>
   </si>
   <si>
-    <t>HealthcareService.notAvailable:closingRepoeningDate.during.start</t>
+    <t>HealthcareService.notAvailable:closingReopeningDate.during.start</t>
   </si>
   <si>
     <t>HealthcareService.notAvailable.during.start</t>
@@ -2056,7 +2056,7 @@
     <t>./low</t>
   </si>
   <si>
-    <t>HealthcareService.notAvailable:closingRepoeningDate.during.end</t>
+    <t>HealthcareService.notAvailable:closingReopeningDate.during.end</t>
   </si>
   <si>
     <t>HealthcareService.notAvailable.during.end</t>

</xml_diff>